<commit_message>
add signature to custom distribution report form. added date created to distribution report base table
</commit_message>
<xml_diff>
--- a/app/config/tables/custom_distribution_reports/forms/custom_distribution_reports/custom_distribution_reports.xlsx
+++ b/app/config/tables/custom_distribution_reports/forms/custom_distribution_reports/custom_distribution_reports.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5040" yWindow="460" windowWidth="28800" windowHeight="16220" tabRatio="994" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" tabRatio="994" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>type</t>
   </si>
@@ -127,13 +127,22 @@
   </si>
   <si>
     <t>skips the finalize screen where the user chooses to save as incomplete or finalized and instead saves as finalized</t>
+  </si>
+  <si>
+    <t>signature</t>
+  </si>
+  <si>
+    <t>Please sign your name to verify this report.</t>
+  </si>
+  <si>
+    <t>receive_signature</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -175,6 +184,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -294,7 +310,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -337,6 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -750,7 +767,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -800,7 +817,15 @@
       <c r="I2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="C3" s="13"/>
+      <c r="A3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>32</v>
+      </c>
       <c r="D3" s="14"/>
       <c r="F3"/>
       <c r="G3"/>
@@ -1028,8 +1053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -1064,7 +1089,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="28">
-        <v>5222017</v>
+        <v>52418</v>
       </c>
       <c r="C3"/>
     </row>
@@ -1096,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1123,7 +1148,7 @@
       <c r="B2" s="35"/>
       <c r="C2" s="35"/>
     </row>
-    <row r="3" spans="1:4" ht="208" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="192" x14ac:dyDescent="0.2">
       <c r="A3" s="35" t="s">
         <v>29</v>
       </c>
@@ -1140,10 +1165,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -1168,6 +1193,14 @@
       </c>
       <c r="B2" s="3" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="36" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>